<commit_message>
finishing books in portuguese
</commit_message>
<xml_diff>
--- a/Selected_Downloads.xlsx
+++ b/Selected_Downloads.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Revistas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Brasil_Pol" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Television" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Brasil_His" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Television" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3079" uniqueCount="3079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3087" uniqueCount="3087">
   <si>
     <t>Index</t>
   </si>
@@ -9252,6 +9253,30 @@
   </si>
   <si>
     <t>Eugenia</t>
+  </si>
+  <si>
+    <t>bub_gb_6d0_7XDSscgC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historia da prouincia sancta Cruz a qui vulgarmente chamamos Brasil feita por Pero de Magalhaens de Gandauo, dirigida ao muito illustre senhor dom Lionis Pereira gouernador que foy di Malaca &amp; das mais partes do sul na India </t>
+  </si>
+  <si>
+    <t>europeanlibraries</t>
+  </si>
+  <si>
+    <t>tools.bub@tools.wmflabs.org</t>
+  </si>
+  <si>
+    <t>bub_upload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-01-15 19:03:42</t>
+  </si>
+  <si>
+    <t>1576</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro : de Magalhaens de Gandavo</t>
   </si>
 </sst>
 </file>
@@ -41414,7 +41439,7 @@
       <c r="B2" s="3" t="s">
         <v>2995</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2996</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -42028,6 +42053,170 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="5.57421875"/>
+    <col customWidth="1" min="3" max="3" width="110.00390625"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3079</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3080</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3081</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>3082</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>3083</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>3084</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>3084</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>3085</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>3086</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
+        <v>3085</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3079</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3080</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3081</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3082</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3083</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>3084</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>3084</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>3085</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>3086</v>
+      </c>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3" t="s">
+        <v>3085</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
adding already skrapped material to the folder
</commit_message>
<xml_diff>
--- a/Selected_Downloads.xlsx
+++ b/Selected_Downloads.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3087" uniqueCount="3087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3095" uniqueCount="3095">
   <si>
     <t>Index</t>
   </si>
@@ -9261,6 +9261,9 @@
     <t xml:space="preserve">Historia da prouincia sancta Cruz a qui vulgarmente chamamos Brasil feita por Pero de Magalhaens de Gandauo, dirigida ao muito illustre senhor dom Lionis Pereira gouernador que foy di Malaca &amp; das mais partes do sul na India </t>
   </si>
   <si>
+    <t>1576</t>
+  </si>
+  <si>
     <t>europeanlibraries</t>
   </si>
   <si>
@@ -9273,22 +9276,49 @@
     <t xml:space="preserve">2016-01-15 19:03:42</t>
   </si>
   <si>
-    <t>1576</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pedro : de Magalhaens de Gandavo</t>
+  </si>
+  <si>
+    <t>or298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diário da Navegação da  Armada que Foi a Terra do Brasil Em 1530 Sob a Capitania-Mor de Martim Affonso de Souza Escripto por seu irmão Pero Lopes de Souza Publicado por  Francisco Adolfo de Varnhagen Lisboa, Typographia da Socieadade Propagadora dos Conhecimentos Úteis 1839</t>
+  </si>
+  <si>
+    <t>1530</t>
+  </si>
+  <si>
+    <t>suiewendhausen@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['Diário da Navegação', 'da  Armada que Foi a Terra do Brasil', 'Em 1530', 'Sob a Capitania-Mor de Martim Affonso de Souza', 'Escripto por seu irmão Pero Lopes de Souza', 'Publicado por  Francisco Adolfo de Varnhagen Lisboa', 'Nau Capitânea', 'Nau San Miguel', 'Galeão São Vicente', 'Caravela Rosa e Caravela Princesa  Dentre as 400 pessoas embarcadas nestes navios', 'poderemos somente mencionar', 'Jorge Pires']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-07-21 19:55:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pero Lopes de Souza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://objdigital.bn.br/objdigital2/acervo_digital/div_obrasraras/or298/or298.pdfDiário da Navegação da Armada que Foi a Terra do BrasilEm 1530 Sob a Capitania-Morde Martim Affonso de SouzaEscripto por seu irmãoPero Lopes de SouzaPublicado por Francisco Adolfo de VarnhagenLisboa, Typographia da Socieadade Propagadora dos Conhecimentos Úteis1839Nau Capitânea, Nau San Miguel, Galeão São Vicente, Caravela Rosa e Caravela PrincesaDentre as 400 pessoas embarcadas nestes navios, poderemos somente mencionar, Jorge Piresobjdigital.bn.br/objdigital2/acervo_digital/div_obrasraras/or298/or298.pdfviar a Portugal, e a seu irmão encarregou do cominan- ... c. p. 243, e um Nobiliário MS» ... tins Ferreira; Pedro Collaço; Jorge Pires; Heitor d'Al-.1.304 páginas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.000000"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -9298,12 +9328,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="2">
@@ -9330,12 +9363,15 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0">
+      <alignment vertical="top"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -9345,12 +9381,11 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -42053,10 +42088,11 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="5.57421875"/>
-    <col customWidth="1" min="3" max="3" width="110.00390625"/>
+    <col customWidth="1" min="3" max="3" width="109.140625"/>
+    <col customWidth="1" min="4" max="4" width="14.00390625"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -42070,28 +42106,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
@@ -42116,28 +42152,28 @@
       <c r="C2" s="3" t="s">
         <v>3080</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3081</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>3082</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>3082</v>
+        <v>21</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>3083</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>3083</v>
+        <v>23</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>3084</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>3084</v>
-      </c>
-      <c r="K2" s="2" t="s">
+        <v>3085</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>3085</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -42145,7 +42181,7 @@
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3" t="s">
-        <v>3085</v>
+        <v>3081</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -42161,31 +42197,31 @@
       <c r="B3" s="3" t="s">
         <v>3079</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3080</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3081</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>3082</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>3082</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>23</v>
+        <v>3083</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>3083</v>
+        <v>23</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>3084</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>3084</v>
-      </c>
-      <c r="K3" s="2" t="s">
+        <v>3085</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>3085</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -42193,7 +42229,7 @@
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3" t="s">
-        <v>3085</v>
+        <v>3081</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
@@ -42202,7 +42238,64 @@
       <c r="S3" s="3"/>
       <c r="T3" s="3"/>
     </row>
+    <row r="4" ht="14.25">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>3087</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>3088</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3089</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3021</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>3090</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>3091</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>3092</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>3092</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>3093</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>3089</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>3094</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="S5"/>
+  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>

<commit_message>
curva abc - janela de tempo 2
</commit_message>
<xml_diff>
--- a/Selected_Downloads.xlsx
+++ b/Selected_Downloads.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4156" uniqueCount="4156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4158" uniqueCount="4158">
   <si>
     <t>Index</t>
   </si>
@@ -12370,6 +12370,27 @@
     <t xml:space="preserve">The Final Conclave</t>
   </si>
   <si>
+    <t xml:space="preserve">An Amazing Journey into the Psychotic Mind - Breaking the Spell of the Ivory Tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jerry Marzinsky</t>
+  </si>
+  <si>
+    <t>Spirituality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Brotherhood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stephen Knight</t>
+  </si>
+  <si>
+    <t>Freemasonry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack the Ripper: The Final Solution</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Brooking Report</t>
   </si>
   <si>
@@ -12439,28 +12460,13 @@
     <t xml:space="preserve">David Rohl</t>
   </si>
   <si>
-    <t xml:space="preserve">An Amazing Journey into the Psychotic Mind - Breaking the Spell of the Ivory Tower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jerry Marzinsky</t>
-  </si>
-  <si>
-    <t>Spirituality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Brotherhood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stephen Knight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jack the Ripper: The Final Solution</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Encyclopedia of Ancient Giants in North America</t>
   </si>
   <si>
     <t xml:space="preserve">Fritz Zimmerman</t>
+  </si>
+  <si>
+    <t>Giants</t>
   </si>
   <si>
     <t xml:space="preserve">Ancient America: The Dark Side</t>
@@ -44661,14 +44667,14 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A117" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" style="11" width="9.140625"/>
-    <col customWidth="1" min="3" max="3" style="11" width="71.421875"/>
+    <col customWidth="1" min="3" max="3" style="11" width="86.7109375"/>
     <col customWidth="1" min="4" max="4" style="11" width="43.8515625"/>
     <col min="5" max="5" style="11" width="9.140625"/>
     <col customWidth="1" min="6" max="6" style="11" width="24.57421875"/>
@@ -46321,293 +46327,371 @@
       <c r="I96" s="11"/>
     </row>
     <row r="97" ht="16.5">
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
+      <c r="C97" s="11" t="s">
+        <v>4113</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>4114</v>
+      </c>
       <c r="E97" s="16"/>
-      <c r="F97" s="11"/>
-    </row>
-    <row r="98" ht="14.25">
-      <c r="C98" s="17"/>
-      <c r="D98" s="11"/>
-      <c r="F98" s="11"/>
+      <c r="F97" s="11" t="s">
+        <v>4115</v>
+      </c>
+    </row>
+    <row r="98" ht="16.5">
+      <c r="C98" s="11" t="s">
+        <v>4116</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>4117</v>
+      </c>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11" t="s">
+        <v>4118</v>
+      </c>
     </row>
     <row r="99" ht="16.5">
-      <c r="C99" s="16" t="s">
-        <v>4113</v>
-      </c>
-      <c r="D99" s="11"/>
-      <c r="F99" s="11"/>
+      <c r="C99" s="11" t="s">
+        <v>4119</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>4117</v>
+      </c>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11" t="s">
+        <v>4118</v>
+      </c>
     </row>
     <row r="100" ht="16.5">
-      <c r="C100" s="16" t="s">
-        <v>4114</v>
-      </c>
+      <c r="C100" s="11"/>
+      <c r="D100" s="16"/>
+      <c r="F100" s="11"/>
     </row>
     <row r="101" ht="16.5">
-      <c r="C101" s="16" t="s">
-        <v>4115</v>
-      </c>
+      <c r="C101" s="11"/>
+      <c r="D101" s="16"/>
+      <c r="F101" s="11"/>
     </row>
     <row r="102" ht="16.5">
-      <c r="C102" s="16" t="s">
-        <v>4116</v>
-      </c>
+      <c r="C102" s="11"/>
+      <c r="D102" s="16"/>
+      <c r="F102" s="11"/>
     </row>
     <row r="103" ht="16.5">
-      <c r="C103" s="16" t="s">
-        <v>4117</v>
-      </c>
+      <c r="C103" s="11"/>
+      <c r="D103" s="16"/>
+      <c r="F103" s="11"/>
     </row>
     <row r="104" ht="16.5">
-      <c r="C104" s="16" t="s">
-        <v>4118</v>
-      </c>
+      <c r="C104" s="11"/>
+      <c r="D104" s="16"/>
+      <c r="F104" s="11"/>
     </row>
     <row r="105" ht="16.5">
-      <c r="C105" s="16" t="s">
-        <v>4119</v>
-      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="16"/>
+      <c r="F105" s="11"/>
     </row>
     <row r="106" ht="16.5">
-      <c r="C106" s="16" t="s">
-        <v>4120</v>
-      </c>
+      <c r="C106" s="11"/>
+      <c r="D106" s="16"/>
+      <c r="F106" s="11"/>
     </row>
     <row r="107" ht="16.5">
-      <c r="C107" s="16" t="s">
-        <v>4121</v>
-      </c>
+      <c r="C107" s="11"/>
+      <c r="D107" s="16"/>
+      <c r="F107" s="11"/>
     </row>
     <row r="108" ht="16.5">
-      <c r="C108" s="16" t="s">
-        <v>4122</v>
-      </c>
+      <c r="C108" s="11"/>
+      <c r="D108" s="16"/>
+      <c r="F108" s="11"/>
     </row>
     <row r="109" ht="16.5">
-      <c r="C109" s="16" t="s">
-        <v>4123</v>
-      </c>
+      <c r="C109" s="11"/>
+      <c r="D109" s="16"/>
+      <c r="F109" s="11"/>
     </row>
     <row r="110" ht="16.5">
-      <c r="C110" s="16" t="s">
-        <v>4124</v>
-      </c>
+      <c r="C110" s="11"/>
+      <c r="D110" s="16"/>
+      <c r="F110" s="11"/>
     </row>
     <row r="111" ht="16.5">
-      <c r="C111" s="16" t="s">
-        <v>4125</v>
-      </c>
+      <c r="C111" s="11"/>
+      <c r="D111" s="16"/>
+      <c r="F111" s="11"/>
     </row>
     <row r="112" ht="16.5">
-      <c r="C112" s="16" t="s">
-        <v>4126</v>
-      </c>
+      <c r="C112" s="11"/>
+      <c r="D112" s="16"/>
+      <c r="F112" s="11"/>
     </row>
     <row r="113" ht="16.5">
-      <c r="C113" s="16" t="s">
-        <v>4127</v>
-      </c>
-      <c r="D113" s="11"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="16"/>
       <c r="F113" s="11"/>
     </row>
     <row r="114" ht="16.5">
-      <c r="C114" s="16" t="s">
-        <v>4128</v>
-      </c>
+      <c r="C114" s="11"/>
+      <c r="D114" s="16"/>
       <c r="F114" s="11"/>
     </row>
-    <row r="115" ht="16.5">
-      <c r="C115" s="16" t="s">
-        <v>4129</v>
-      </c>
+    <row r="115" ht="14.25">
+      <c r="C115" s="17"/>
+      <c r="D115" s="11"/>
       <c r="F115" s="11"/>
     </row>
     <row r="116" ht="16.5">
       <c r="C116" s="16" t="s">
-        <v>4130</v>
-      </c>
+        <v>4120</v>
+      </c>
+      <c r="D116" s="11"/>
       <c r="F116" s="11"/>
     </row>
     <row r="117" ht="16.5">
       <c r="C117" s="16" t="s">
-        <v>4131</v>
+        <v>4121</v>
       </c>
     </row>
     <row r="118" ht="16.5">
-      <c r="C118" s="19" t="s">
-        <v>4132</v>
-      </c>
-    </row>
-    <row r="119" ht="14.25"/>
+      <c r="C118" s="16" t="s">
+        <v>4122</v>
+      </c>
+    </row>
+    <row r="119" ht="16.5">
+      <c r="C119" s="16" t="s">
+        <v>4123</v>
+      </c>
+    </row>
     <row r="120" ht="16.5">
       <c r="C120" s="16" t="s">
-        <v>4133</v>
+        <v>4124</v>
       </c>
     </row>
     <row r="121" ht="16.5">
-      <c r="C121" s="11"/>
-      <c r="D121" s="11"/>
+      <c r="C121" s="16" t="s">
+        <v>4125</v>
+      </c>
     </row>
     <row r="122" ht="16.5">
       <c r="C122" s="16" t="s">
-        <v>4134</v>
-      </c>
-      <c r="D122" s="11"/>
-      <c r="F122" s="11"/>
+        <v>4126</v>
+      </c>
     </row>
     <row r="123" ht="16.5">
       <c r="C123" s="16" t="s">
+        <v>4127</v>
+      </c>
+    </row>
+    <row r="124" ht="16.5">
+      <c r="C124" s="16" t="s">
+        <v>4128</v>
+      </c>
+    </row>
+    <row r="125" ht="16.5">
+      <c r="C125" s="16" t="s">
+        <v>4129</v>
+      </c>
+    </row>
+    <row r="126" ht="16.5">
+      <c r="C126" s="16" t="s">
+        <v>4130</v>
+      </c>
+    </row>
+    <row r="127" ht="16.5">
+      <c r="C127" s="16" t="s">
+        <v>4131</v>
+      </c>
+    </row>
+    <row r="128" ht="16.5">
+      <c r="C128" s="16" t="s">
+        <v>4132</v>
+      </c>
+    </row>
+    <row r="129" ht="16.5">
+      <c r="C129" s="16" t="s">
+        <v>4133</v>
+      </c>
+    </row>
+    <row r="130" ht="16.5">
+      <c r="C130" s="16" t="s">
+        <v>4134</v>
+      </c>
+      <c r="D130" s="11"/>
+      <c r="F130" s="11"/>
+    </row>
+    <row r="131" ht="16.5">
+      <c r="C131" s="16" t="s">
         <v>4135</v>
       </c>
-      <c r="D123" s="11"/>
-    </row>
-    <row r="124" ht="16.5">
-      <c r="C124" s="11"/>
-      <c r="F124" s="11"/>
-    </row>
-    <row r="125" ht="16.5">
-      <c r="C125" s="11" t="s">
+      <c r="F131" s="11"/>
+    </row>
+    <row r="132" ht="16.5">
+      <c r="C132" s="16" t="s">
         <v>4136</v>
       </c>
-      <c r="D125" s="11" t="s">
+      <c r="F132" s="11"/>
+    </row>
+    <row r="133" ht="16.5">
+      <c r="C133" s="16" t="s">
         <v>4137</v>
       </c>
-      <c r="E125" s="16"/>
-      <c r="F125" s="11" t="s">
+      <c r="F133" s="11"/>
+    </row>
+    <row r="134" ht="16.5">
+      <c r="C134" s="16" t="s">
         <v>4138</v>
       </c>
-    </row>
-    <row r="126" ht="16.5"/>
-    <row r="127" ht="16.5"/>
-    <row r="128" ht="16.5"/>
-    <row r="129" ht="16.5"/>
-    <row r="130" ht="16.5">
-      <c r="F130" s="11"/>
-    </row>
-    <row r="131" ht="16.5">
-      <c r="F131" s="11"/>
-    </row>
-    <row r="133" ht="16.5">
-      <c r="C133" s="11" t="s">
+      <c r="F134" s="11"/>
+    </row>
+    <row r="135" ht="16.5">
+      <c r="C135" s="19" t="s">
         <v>4139</v>
       </c>
-      <c r="D133" s="16" t="s">
+    </row>
+    <row r="136" ht="14.25"/>
+    <row r="137" ht="16.5">
+      <c r="C137" s="16" t="s">
         <v>4140</v>
       </c>
     </row>
-    <row r="134" ht="16.5">
-      <c r="C134" s="11" t="s">
+    <row r="138" ht="16.5">
+      <c r="C138" s="11"/>
+      <c r="D138" s="11"/>
+      <c r="E138" s="11"/>
+    </row>
+    <row r="139" ht="16.5">
+      <c r="C139" s="16" t="s">
         <v>4141</v>
       </c>
-      <c r="D134" s="16" t="s">
-        <v>4140</v>
-      </c>
-      <c r="F134" s="11"/>
-    </row>
-    <row r="135" ht="14.25">
-      <c r="C135" s="11"/>
-      <c r="D135" s="11"/>
-      <c r="F135" s="11"/>
-    </row>
-    <row r="136" ht="14.25">
-      <c r="C136" s="11"/>
-      <c r="D136" s="11"/>
-      <c r="F136" s="11"/>
-    </row>
-    <row r="137" ht="14.25"/>
-    <row r="138" ht="16.5">
-      <c r="C138" s="11" t="s">
+      <c r="D139" s="11"/>
+      <c r="E139" s="11"/>
+      <c r="F139" s="11"/>
+    </row>
+    <row r="140" ht="16.5">
+      <c r="C140" s="16" t="s">
         <v>4142</v>
       </c>
-      <c r="D138" s="11" t="s">
+      <c r="D140" s="11"/>
+      <c r="E140" s="11"/>
+    </row>
+    <row r="141" ht="16.5">
+      <c r="C141" s="11"/>
+      <c r="E141" s="11"/>
+      <c r="F141" s="11"/>
+    </row>
+    <row r="142" ht="16.5">
+      <c r="F142" s="11"/>
+    </row>
+    <row r="143" ht="14.25"/>
+    <row r="144" ht="16.5">
+      <c r="C144" s="11" t="s">
         <v>4143</v>
       </c>
-    </row>
-    <row r="139" ht="16.5">
-      <c r="C139" s="11" t="s">
+      <c r="D144" s="11" t="s">
         <v>4144</v>
       </c>
-      <c r="D139" s="11" t="s">
-        <v>4143</v>
-      </c>
-    </row>
-    <row r="140" ht="16.5">
-      <c r="C140" s="11" t="s">
+      <c r="F144" s="11" t="s">
         <v>4145</v>
       </c>
-      <c r="D140" s="11" t="s">
-        <v>4143</v>
-      </c>
-    </row>
-    <row r="141" ht="16.5">
-      <c r="C141" s="11" t="s">
+    </row>
+    <row r="145" ht="16.5">
+      <c r="C145" s="11" t="s">
         <v>4146</v>
       </c>
-      <c r="D141" s="11" t="s">
+      <c r="D145" s="11" t="s">
+        <v>4144</v>
+      </c>
+      <c r="F145" s="11" t="s">
+        <v>4145</v>
+      </c>
+    </row>
+    <row r="146" ht="16.5">
+      <c r="C146" s="11" t="s">
         <v>4147</v>
       </c>
-    </row>
-    <row r="142" ht="16.5">
-      <c r="C142" s="11" t="s">
+      <c r="D146" s="11" t="s">
+        <v>4144</v>
+      </c>
+      <c r="F146" s="11" t="s">
+        <v>4145</v>
+      </c>
+    </row>
+    <row r="147" ht="16.5">
+      <c r="C147" s="11" t="s">
         <v>4148</v>
       </c>
-      <c r="D142" s="11" t="s">
+      <c r="D147" s="11" t="s">
+        <v>4149</v>
+      </c>
+      <c r="F147" s="11" t="s">
+        <v>4145</v>
+      </c>
+    </row>
+    <row r="148" ht="16.5">
+      <c r="C148" s="11" t="s">
+        <v>4150</v>
+      </c>
+      <c r="F148" s="11" t="s">
         <v>4053</v>
       </c>
-      <c r="F142" s="11"/>
-    </row>
-    <row r="143" ht="14.25">
-      <c r="C143" s="11"/>
-      <c r="D143" s="11"/>
-      <c r="F143" s="11"/>
-    </row>
-    <row r="146" ht="16.5">
-      <c r="C146" s="21" t="s">
-        <v>4149</v>
-      </c>
-      <c r="D146" s="11" t="s">
-        <v>4150</v>
-      </c>
-    </row>
-    <row r="148" ht="14.25"/>
-    <row r="149" ht="16.5">
-      <c r="C149" s="11" t="s">
+    </row>
+    <row r="149" ht="14.25">
+      <c r="C149" s="11"/>
+      <c r="D149" s="11"/>
+      <c r="F149" s="11"/>
+    </row>
+    <row r="152" ht="16.5">
+      <c r="C152" s="21" t="s">
         <v>4151</v>
       </c>
-    </row>
-    <row r="150" ht="16.5">
-      <c r="C150" s="11" t="s">
+      <c r="D152" s="11" t="s">
         <v>4152</v>
       </c>
-    </row>
-    <row r="151" ht="14.25"/>
-    <row r="152" ht="16.5"/>
-    <row r="153" ht="14.25"/>
-    <row r="154" ht="14.25">
-      <c r="C154" s="11"/>
-      <c r="D154" s="11"/>
-      <c r="F154" s="11"/>
-    </row>
-    <row r="156" ht="16.5"/>
-    <row r="157" ht="16.5">
-      <c r="C157" s="11"/>
-      <c r="D157" s="11"/>
-    </row>
-    <row r="162" ht="16.5">
-      <c r="C162" s="11" t="s">
+      <c r="F152" s="11"/>
+    </row>
+    <row r="153" ht="14.25">
+      <c r="C153" s="11"/>
+      <c r="D153" s="11"/>
+      <c r="F153" s="11"/>
+    </row>
+    <row r="154" ht="14.25"/>
+    <row r="155" ht="16.5">
+      <c r="C155" s="11" t="s">
         <v>4153</v>
       </c>
-      <c r="D162" s="11" t="s">
+    </row>
+    <row r="156" ht="16.5">
+      <c r="C156" s="11" t="s">
         <v>4154</v>
       </c>
     </row>
-    <row r="169" ht="16.5">
-      <c r="C169" s="11" t="s">
+    <row r="157" ht="14.25"/>
+    <row r="158" ht="16.5">
+      <c r="C158" s="11" t="s">
         <v>4155</v>
       </c>
-      <c r="D169" s="11" t="s">
+      <c r="D158" s="11" t="s">
+        <v>4156</v>
+      </c>
+    </row>
+    <row r="159" ht="16.5">
+      <c r="C159" s="11" t="s">
+        <v>4157</v>
+      </c>
+      <c r="D159" s="11" t="s">
         <v>3991</v>
       </c>
+    </row>
+    <row r="160" ht="14.25">
+      <c r="C160" s="11"/>
+      <c r="D160" s="11"/>
+      <c r="F160" s="11"/>
+    </row>
+    <row r="163" ht="14.25">
+      <c r="C163" s="11"/>
+      <c r="D163" s="11"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>

</xml_diff>